<commit_message>
all issues with lps resolved, also added the ema for lp
</commit_message>
<xml_diff>
--- a/run_merged.xlsx
+++ b/run_merged.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO22"/>
+  <dimension ref="A1:AM22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,155 +469,145 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>max_pnl_traders</t>
+          <t>oi_long_btc</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>min_pnl_traders</t>
+          <t>oi_long_eth</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>oi_long_btc</t>
+          <t>oi_long_sol</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>oi_long_eth</t>
+          <t>oi_short_btc</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>oi_long_sol</t>
+          <t>oi_short_eth</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>oi_short_btc</t>
+          <t>oi_short_sol</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>oi_short_eth</t>
+          <t>volume_btc</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>oi_short_sol</t>
+          <t>volume_eth</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>volume_btc</t>
+          <t>volume_sol</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>volume_eth</t>
+          <t>num_of_longs</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>volume_sol</t>
+          <t>num_of_shorts</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>num_of_longs</t>
+          <t>num_of_swaps</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>num_of_shorts</t>
+          <t>number_of_liquidations</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>num_of_swaps</t>
+          <t>fees_collected_btc</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>number_of_liquidations</t>
+          <t>fees_collected_eth</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>fees_collected_btc</t>
+          <t>fees_collected_sol</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>fees_collected_eth</t>
+          <t>fees_collected_usdc</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>fees_collected_sol</t>
+          <t>fees_collected_usdt</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>fees_collected_usdc</t>
+          <t>treasury_balance_btc</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>fees_collected_usdt</t>
+          <t>treasury_balance_eth</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>treasury_balance_btc</t>
+          <t>treasury_balance_sol</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>treasury_balance_eth</t>
+          <t>treasury_balance_usdc</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>treasury_balance_sol</t>
+          <t>treasury_balance_usdt</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>treasury_balance_usdc</t>
+          <t>pool_pnl_btc</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>treasury_balance_usdt</t>
+          <t>pool_pnl_eth</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>pool_pnl_btc</t>
+          <t>pool_pnl_sol</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>pool_pnl_eth</t>
+          <t>nominal_exposure_btc</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>pool_pnl_sol</t>
+          <t>nominal_exposure_eth</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
-        <is>
-          <t>nominal_exposure_btc</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>nominal_exposure_eth</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
         <is>
           <t>nominal_exposure_sol</t>
         </is>
@@ -632,7 +622,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="n">
         <v>100</v>
@@ -740,12 +730,6 @@
         <v>0</v>
       </c>
       <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -757,121 +741,115 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>100.5038749224246</v>
+        <v>100.1718868073973</v>
       </c>
       <c r="E4" t="n">
-        <v>10.11807814883019</v>
+        <v>9.939631349722204</v>
       </c>
       <c r="F4" t="n">
-        <v>111.1747263542306</v>
+        <v>109.9574176448915</v>
       </c>
       <c r="G4" t="n">
-        <v>2548.488906184862</v>
+        <v>2514.462741805661</v>
       </c>
       <c r="H4" t="n">
-        <v>451663.736064829</v>
+        <v>451326.202615164</v>
       </c>
       <c r="I4" t="n">
-        <v>447847.7912283594</v>
+        <v>452864.848444538</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>1.101520210866781</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>3.736803748348708</v>
       </c>
       <c r="M4" t="n">
-        <v>3.695797777801049</v>
+        <v>127.6529764002356</v>
       </c>
       <c r="N4" t="n">
-        <v>8.771328380189402</v>
+        <v>2.735017553013878</v>
       </c>
       <c r="O4" t="n">
-        <v>181.2270753516281</v>
+        <v>9.058681744216099</v>
       </c>
       <c r="P4" t="n">
-        <v>1.31443716032748</v>
+        <v>90.10426667040268</v>
       </c>
       <c r="Q4" t="n">
-        <v>12.67832574088475</v>
+        <v>3.836537763880659</v>
       </c>
       <c r="R4" t="n">
-        <v>106.0821953322296</v>
+        <v>12.79548549256481</v>
       </c>
       <c r="S4" t="n">
-        <v>5.010234938128528</v>
+        <v>217.7572430706383</v>
       </c>
       <c r="T4" t="n">
-        <v>21.44965412107415</v>
+        <v>11</v>
       </c>
       <c r="U4" t="n">
-        <v>287.3092706838577</v>
+        <v>17</v>
       </c>
       <c r="V4" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="W4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>36</v>
+        <v>0.07266105328916221</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>0.0732637229270732</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.08086431416176021</v>
+        <v>0.166124544865536</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2549342231641614</v>
+        <v>0.09780425765775048</v>
       </c>
       <c r="AB4" t="n">
-        <v>22.89603443582947</v>
+        <v>0.09722767695248953</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.09760924222876936</v>
+        <v>0.02220162146747567</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1083420215846238</v>
+        <v>0.02223846083313241</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.02445490241455321</v>
+        <v>0.049609623658357</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.07689170131331147</v>
+        <v>0.02907107116537775</v>
       </c>
       <c r="AG4" t="n">
-        <v>7.039449650986731</v>
+        <v>0.02907474064713209</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.02907096095010844</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.03213218257412859</v>
+        <v>0</v>
       </c>
       <c r="AJ4" t="n">
         <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>0</v>
+        <v>0.7145418145923162</v>
       </c>
       <c r="AL4" t="n">
-        <v>0</v>
+        <v>1.34128240152977</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.38136061747357</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>-3.906997360695346</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>75.1448800193984</v>
+        <v>127.3621378219362</v>
       </c>
     </row>
     <row r="5">
@@ -882,121 +860,115 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>100.8578034843422</v>
+        <v>100.3902140464563</v>
       </c>
       <c r="E5" t="n">
-        <v>10.45764914110724</v>
+        <v>10.21407544704054</v>
       </c>
       <c r="F5" t="n">
-        <v>110.489113628202</v>
+        <v>109.8190534548452</v>
       </c>
       <c r="G5" t="n">
-        <v>2561.3741108965</v>
+        <v>2475.258801136957</v>
       </c>
       <c r="H5" t="n">
-        <v>446137.6270610343</v>
+        <v>442954.0022520028</v>
       </c>
       <c r="I5" t="n">
-        <v>451633.2858106701</v>
+        <v>462783.9696437969</v>
       </c>
       <c r="J5" t="n">
-        <v>-4277.498100256402</v>
+        <v>-2280.804013834905</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.1130761561470324</v>
       </c>
       <c r="L5" t="n">
-        <v>-4277.498100256402</v>
+        <v>15.11817169076729</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9915712321704322</v>
+        <v>362.0613552693769</v>
       </c>
       <c r="N5" t="n">
-        <v>13.50403414239744</v>
+        <v>5.101048165625524</v>
       </c>
       <c r="O5" t="n">
-        <v>181.2270753516281</v>
+        <v>22.89455488466527</v>
       </c>
       <c r="P5" t="n">
-        <v>5.549329258979967</v>
+        <v>500.3502579779669</v>
       </c>
       <c r="Q5" t="n">
-        <v>32.1728416789374</v>
+        <v>6.26303549026311</v>
       </c>
       <c r="R5" t="n">
-        <v>285.0719561747729</v>
+        <v>38.01272657543256</v>
       </c>
       <c r="S5" t="n">
-        <v>9.261044086584025</v>
+        <v>974.3606916496295</v>
       </c>
       <c r="T5" t="n">
-        <v>45.67687582133484</v>
+        <v>23</v>
       </c>
       <c r="U5" t="n">
-        <v>466.299031526401</v>
+        <v>40</v>
       </c>
       <c r="V5" t="n">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="W5" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="X5" t="n">
-        <v>68</v>
+        <v>0.1646070720827982</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>0.1272280279690226</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.1858512467084233</v>
+        <v>1.304090032188522</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.4064293718537779</v>
+        <v>0.23653815675622</v>
       </c>
       <c r="AB5" t="n">
-        <v>23.25351163035842</v>
+        <v>0.190060942102739</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1795414847496317</v>
+        <v>0.05031349280634892</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.2224484040932233</v>
+        <v>0.03868219656877168</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.05621685211214349</v>
+        <v>0.3964957891417679</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.12280278252807</v>
+        <v>0.07038789901957594</v>
       </c>
       <c r="AG5" t="n">
-        <v>7.371753908501186</v>
+        <v>0.0566119015005908</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.05355365748697945</v>
+        <v>-141.2551137639337</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.06579282283549472</v>
+        <v>-0.3789436764211835</v>
       </c>
       <c r="AJ5" t="n">
-        <v>4125.653798783726</v>
+        <v>139.457121363117</v>
       </c>
       <c r="AK5" t="n">
-        <v>0</v>
+        <v>-1.072870264446151</v>
       </c>
       <c r="AL5" t="n">
-        <v>0</v>
+        <v>9.359656928301767</v>
       </c>
       <c r="AM5" t="n">
-        <v>-4.557758026809535</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>-18.66880753653996</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>-103.8448808231449</v>
+        <v>188.9951779092583</v>
       </c>
     </row>
     <row r="6">
@@ -1007,121 +979,115 @@
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>101.2719181877742</v>
+        <v>100.6332218261952</v>
       </c>
       <c r="E6" t="n">
-        <v>10.54119311182859</v>
+        <v>10.33127060712746</v>
       </c>
       <c r="F6" t="n">
-        <v>112.2056580454612</v>
+        <v>109.8670192149424</v>
       </c>
       <c r="G6" t="n">
-        <v>2589.927822028417</v>
+        <v>2465.754510020412</v>
       </c>
       <c r="H6" t="n">
-        <v>445005.7348314032</v>
+        <v>445476.5589155392</v>
       </c>
       <c r="I6" t="n">
-        <v>451920.0092806926</v>
+        <v>463258.8763198786</v>
       </c>
       <c r="J6" t="n">
-        <v>-4399.492419751371</v>
+        <v>-4029.661383742764</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.6354793316611387</v>
       </c>
       <c r="L6" t="n">
-        <v>-4277.498100256402</v>
+        <v>24.14853462951258</v>
       </c>
       <c r="M6" t="n">
-        <v>2.504029210352961</v>
+        <v>183.1672924758572</v>
       </c>
       <c r="N6" t="n">
-        <v>25.55256171300445</v>
+        <v>5.606635782032344</v>
       </c>
       <c r="O6" t="n">
-        <v>289.5847053534504</v>
+        <v>37.91966154996389</v>
       </c>
       <c r="P6" t="n">
-        <v>5.657025074305915</v>
+        <v>628.7121027601667</v>
       </c>
       <c r="Q6" t="n">
-        <v>54.63475443201452</v>
+        <v>7.528763809942165</v>
       </c>
       <c r="R6" t="n">
-        <v>435.5269432621341</v>
+        <v>62.06819617947647</v>
       </c>
       <c r="S6" t="n">
-        <v>11.05224163049833</v>
+        <v>1143.455199699523</v>
       </c>
       <c r="T6" t="n">
-        <v>80.18731614501895</v>
+        <v>37</v>
       </c>
       <c r="U6" t="n">
-        <v>735.1454407755605</v>
+        <v>53</v>
       </c>
       <c r="V6" t="n">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="W6" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="X6" t="n">
-        <v>96</v>
+        <v>0.2340453460297094</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>0.2013495682456583</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.2535767609890874</v>
+        <v>3.658695127334135</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.7798255702764892</v>
+        <v>84.07752152729427</v>
       </c>
       <c r="AB6" t="n">
-        <v>40.14016276235348</v>
+        <v>0.2726505548520815</v>
       </c>
       <c r="AC6" t="n">
-        <v>25.30843856709421</v>
+        <v>0.07119177382885987</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.2997633766296724</v>
+        <v>0.0614898015176601</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.07707827499045765</v>
+        <v>1.125999038584667</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.2350497695460159</v>
+        <v>20.44625953475862</v>
       </c>
       <c r="AG6" t="n">
-        <v>12.56825780703151</v>
+        <v>0.08109501358835343</v>
       </c>
       <c r="AH6" t="n">
-        <v>8.418478667810056</v>
+        <v>-11.55990264952152</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.0887443282664772</v>
+        <v>-64.53919592395798</v>
       </c>
       <c r="AJ6" t="n">
-        <v>319.8237624822477</v>
+        <v>98.64294955242906</v>
       </c>
       <c r="AK6" t="n">
-        <v>109.1025722873237</v>
+        <v>-1.052308173048381</v>
       </c>
       <c r="AL6" t="n">
-        <v>273.2415585337737</v>
+        <v>3.55768686663372</v>
       </c>
       <c r="AM6" t="n">
-        <v>-3.152995863952954</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>-29.08219271901006</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>-145.9422379086837</v>
+        <v>-112.3318929250445</v>
       </c>
     </row>
     <row r="7">
@@ -1132,121 +1098,115 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>101.5844987060325</v>
+        <v>101.14071188752</v>
       </c>
       <c r="E7" t="n">
-        <v>10.65757106413156</v>
+        <v>10.45642238430333</v>
       </c>
       <c r="F7" t="n">
-        <v>111.9703186481133</v>
+        <v>110.5986337468933</v>
       </c>
       <c r="G7" t="n">
-        <v>2685.615892297833</v>
+        <v>2474.030945108719</v>
       </c>
       <c r="H7" t="n">
-        <v>442870.3518273953</v>
+        <v>452240.8270113819</v>
       </c>
       <c r="I7" t="n">
-        <v>450177.462531301</v>
+        <v>462443.6330119895</v>
       </c>
       <c r="J7" t="n">
-        <v>-11992.24467248126</v>
+        <v>-9087.258186410001</v>
       </c>
       <c r="K7" t="n">
-        <v>741.8960355270235</v>
+        <v>0.6349366355401747</v>
       </c>
       <c r="L7" t="n">
-        <v>-4277.498100256402</v>
+        <v>11.00285975726768</v>
       </c>
       <c r="M7" t="n">
-        <v>2.2978348350635</v>
+        <v>283.743505157293</v>
       </c>
       <c r="N7" t="n">
-        <v>23.74263446454054</v>
+        <v>5.964933332942397</v>
       </c>
       <c r="O7" t="n">
-        <v>110.4450142574586</v>
+        <v>37.07277374616351</v>
       </c>
       <c r="P7" t="n">
-        <v>5.953937133217829</v>
+        <v>647.8921882371452</v>
       </c>
       <c r="Q7" t="n">
-        <v>57.94960114583318</v>
+        <v>8.482778837219728</v>
       </c>
       <c r="R7" t="n">
-        <v>528.2285272179025</v>
+        <v>67.21358216785231</v>
       </c>
       <c r="S7" t="n">
-        <v>12.65058624725298</v>
+        <v>1263.211497857937</v>
       </c>
       <c r="T7" t="n">
-        <v>84.44091094186705</v>
+        <v>49</v>
       </c>
       <c r="U7" t="n">
-        <v>856.1780228591284</v>
+        <v>65</v>
       </c>
       <c r="V7" t="n">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="W7" t="n">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="X7" t="n">
-        <v>130</v>
+        <v>0.3277660027762958</v>
       </c>
       <c r="Y7" t="n">
-        <v>5</v>
+        <v>0.4457693563290898</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.3466136111577209</v>
+        <v>3.927490961986821</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.9128960031689167</v>
+        <v>217.3832213614502</v>
       </c>
       <c r="AB7" t="n">
-        <v>44.27844388767873</v>
+        <v>0.3341706578580207</v>
       </c>
       <c r="AC7" t="n">
-        <v>86.7966701196443</v>
+        <v>0.09914882719049257</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.3563604285394941</v>
+        <v>0.1359501763368433</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.1051632586324427</v>
+        <v>1.23326388416067</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.2752135508018545</v>
+        <v>89.52956680546281</v>
       </c>
       <c r="AG7" t="n">
-        <v>13.83211815113002</v>
+        <v>0.09953277589457844</v>
       </c>
       <c r="AH7" t="n">
-        <v>30.40487321589165</v>
+        <v>27.86931858836749</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.1055803577466779</v>
+        <v>2223.885972905823</v>
       </c>
       <c r="AJ7" t="n">
-        <v>592.2841464814337</v>
+        <v>-156.1471722834308</v>
       </c>
       <c r="AK7" t="n">
-        <v>984.079335611752</v>
+        <v>-1.38975612587275</v>
       </c>
       <c r="AL7" t="n">
-        <v>-79.9448172036241</v>
+        <v>-8.741100201810792</v>
       </c>
       <c r="AM7" t="n">
-        <v>-3.656102298154329</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>-34.20696668129263</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>-417.783512960444</v>
+        <v>-30.93576572058721</v>
       </c>
     </row>
     <row r="8">
@@ -1257,121 +1217,115 @@
         <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>102.0953650342726</v>
+        <v>101.4285463720905</v>
       </c>
       <c r="E8" t="n">
-        <v>10.83127388273225</v>
+        <v>10.37834105298256</v>
       </c>
       <c r="F8" t="n">
-        <v>113.1074670257101</v>
+        <v>110.6002534765961</v>
       </c>
       <c r="G8" t="n">
-        <v>2715.019791249013</v>
+        <v>2509.535533454152</v>
       </c>
       <c r="H8" t="n">
-        <v>433344.3841948528</v>
+        <v>461020.6155450159</v>
       </c>
       <c r="I8" t="n">
-        <v>458079.9116801339</v>
+        <v>463617.2808217652</v>
       </c>
       <c r="J8" t="n">
-        <v>-12743.44662942632</v>
+        <v>-14699.7761779233</v>
       </c>
       <c r="K8" t="n">
-        <v>3992.519515601797</v>
+        <v>0.9538171095177974</v>
       </c>
       <c r="L8" t="n">
-        <v>-4277.498100256402</v>
+        <v>8.705567463541611</v>
       </c>
       <c r="M8" t="n">
-        <v>1.667356696992079</v>
+        <v>110.1104569858712</v>
       </c>
       <c r="N8" t="n">
-        <v>23.46686750594201</v>
+        <v>6.103553169399076</v>
       </c>
       <c r="O8" t="n">
-        <v>110.4450142574586</v>
+        <v>46.82423990485397</v>
       </c>
       <c r="P8" t="n">
-        <v>6.161082089220478</v>
+        <v>745.8838868868154</v>
       </c>
       <c r="Q8" t="n">
-        <v>64.12366515903121</v>
+        <v>8.96103337073135</v>
       </c>
       <c r="R8" t="n">
-        <v>539.3972553961612</v>
+        <v>79.1518032022922</v>
       </c>
       <c r="S8" t="n">
-        <v>13.38236397226087</v>
+        <v>1466.211787051586</v>
       </c>
       <c r="T8" t="n">
-        <v>112.7276102005701</v>
+        <v>61</v>
       </c>
       <c r="U8" t="n">
-        <v>937.1515403374776</v>
+        <v>81</v>
       </c>
       <c r="V8" t="n">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="W8" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="X8" t="n">
-        <v>158</v>
+        <v>0.3697220553787011</v>
       </c>
       <c r="Y8" t="n">
-        <v>9</v>
+        <v>0.5144227286199403</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.4233707236960015</v>
+        <v>5.893912415536763</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.304865746036751</v>
+        <v>348.4832155066746</v>
       </c>
       <c r="AB8" t="n">
-        <v>45.24256782067147</v>
+        <v>28.32415817323481</v>
       </c>
       <c r="AC8" t="n">
-        <v>691.6033720698458</v>
+        <v>0.1119593825162937</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.4178002604217553</v>
+        <v>0.1564770723439879</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.1282791020845142</v>
+        <v>1.836274469965516</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.3925873129221939</v>
+        <v>142.4357847173075</v>
       </c>
       <c r="AG8" t="n">
-        <v>14.75104195946574</v>
+        <v>4.367724053197215</v>
       </c>
       <c r="AH8" t="n">
-        <v>30.67718856098115</v>
+        <v>78.19330338523127</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.1239595732982045</v>
+        <v>128.6027695010023</v>
       </c>
       <c r="AJ8" t="n">
-        <v>-6871.735813806343</v>
+        <v>-1180.339453171759</v>
       </c>
       <c r="AK8" t="n">
-        <v>165.7062324288991</v>
+        <v>-1.052305371834049</v>
       </c>
       <c r="AL8" t="n">
-        <v>-1640.308329576927</v>
+        <v>-18.60583084192604</v>
       </c>
       <c r="AM8" t="n">
-        <v>-4.493725392228399</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>-40.6567976530892</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>-428.9522411387027</v>
+        <v>-258.8776983716772</v>
       </c>
     </row>
     <row r="9">
@@ -1382,121 +1336,115 @@
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>102.3953384538224</v>
+        <v>101.6725425040968</v>
       </c>
       <c r="E9" t="n">
-        <v>10.84381265331796</v>
+        <v>10.44279086497219</v>
       </c>
       <c r="F9" t="n">
-        <v>115.0696604927492</v>
+        <v>110.6931289347869</v>
       </c>
       <c r="G9" t="n">
-        <v>2759.228242515</v>
+        <v>2519.643190221271</v>
       </c>
       <c r="H9" t="n">
-        <v>433251.2443782678</v>
+        <v>455868.9821558222</v>
       </c>
       <c r="I9" t="n">
-        <v>454265.4581058427</v>
+        <v>468368.6721378226</v>
       </c>
       <c r="J9" t="n">
-        <v>-14938.27268159434</v>
+        <v>-13891.76040177088</v>
       </c>
       <c r="K9" t="n">
-        <v>3992.519515601797</v>
+        <v>0.9692591045932942</v>
       </c>
       <c r="L9" t="n">
-        <v>-5459.990614522182</v>
+        <v>7.995453113466611</v>
       </c>
       <c r="M9" t="n">
-        <v>1.952357359876112</v>
+        <v>467.3181621623786</v>
       </c>
       <c r="N9" t="n">
-        <v>13.49753453910545</v>
+        <v>6.04983661127886</v>
       </c>
       <c r="O9" t="n">
-        <v>108.3576300018224</v>
+        <v>41.23637670551631</v>
       </c>
       <c r="P9" t="n">
-        <v>6.007029466666603</v>
+        <v>563.8739281247398</v>
       </c>
       <c r="Q9" t="n">
-        <v>100.9432733416993</v>
+        <v>9.493182895788557</v>
       </c>
       <c r="R9" t="n">
-        <v>417.6646904885336</v>
+        <v>88.64361970533142</v>
       </c>
       <c r="S9" t="n">
-        <v>14.30821380962374</v>
+        <v>1855.061025288403</v>
       </c>
       <c r="T9" t="n">
-        <v>149.8819292545149</v>
+        <v>67</v>
       </c>
       <c r="U9" t="n">
-        <v>971.9955013375551</v>
+        <v>87</v>
       </c>
       <c r="V9" t="n">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="W9" t="n">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="X9" t="n">
-        <v>184</v>
+        <v>0.4195182621848692</v>
       </c>
       <c r="Y9" t="n">
-        <v>12</v>
+        <v>0.5712302431974036</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.4524396753758522</v>
+        <v>7.289515384293621</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.491272119891306</v>
+        <v>1060.869655054211</v>
       </c>
       <c r="AB9" t="n">
-        <v>45.30945031963169</v>
+        <v>86.70939795008394</v>
       </c>
       <c r="AC9" t="n">
-        <v>1057.146821188201</v>
+        <v>0.1277262647481623</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5049321869429575</v>
+        <v>0.173979832332374</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.1371106641991467</v>
+        <v>2.257043287683219</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.4481832724694113</v>
+        <v>143.0663294189294</v>
       </c>
       <c r="AG9" t="n">
-        <v>14.77117098304017</v>
+        <v>36.03721227080098</v>
       </c>
       <c r="AH9" t="n">
-        <v>76.8986381367109</v>
+        <v>1552.49330381935</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.1498355582241548</v>
+        <v>-17.46729589497636</v>
       </c>
       <c r="AJ9" t="n">
-        <v>-9784.736263997595</v>
+        <v>-871.0090097166656</v>
       </c>
       <c r="AK9" t="n">
-        <v>-2509.639280873591</v>
+        <v>-0.9831468186383355</v>
       </c>
       <c r="AL9" t="n">
-        <v>-416.533522547718</v>
+        <v>-4.455020161251017</v>
       </c>
       <c r="AM9" t="n">
-        <v>-4.05467210679049</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>-87.44573880259387</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>-309.3070604867113</v>
+        <v>280.3399655669057</v>
       </c>
     </row>
     <row r="10">
@@ -1507,121 +1455,115 @@
         <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>102.6874794508211</v>
+        <v>101.8664660947523</v>
       </c>
       <c r="E10" t="n">
-        <v>10.97681793032261</v>
+        <v>10.5941041169611</v>
       </c>
       <c r="F10" t="n">
-        <v>114.8040814783402</v>
+        <v>113.2703723373382</v>
       </c>
       <c r="G10" t="n">
-        <v>2781.569922337187</v>
+        <v>2510.685052926541</v>
       </c>
       <c r="H10" t="n">
-        <v>429890.3978247565</v>
+        <v>453681.2477834333</v>
       </c>
       <c r="I10" t="n">
-        <v>455078.7480375116</v>
+        <v>469178.4145282091</v>
       </c>
       <c r="J10" t="n">
-        <v>-10970.97049396925</v>
+        <v>-22077.79325266708</v>
       </c>
       <c r="K10" t="n">
-        <v>8356.403123553539</v>
+        <v>0.4408284791810788</v>
       </c>
       <c r="L10" t="n">
-        <v>-5663.323048066535</v>
+        <v>5.567901400886226</v>
       </c>
       <c r="M10" t="n">
-        <v>2.310177559831165</v>
+        <v>122.0232158536792</v>
       </c>
       <c r="N10" t="n">
-        <v>10.95278595287182</v>
+        <v>6.464215598908367</v>
       </c>
       <c r="O10" t="n">
-        <v>167.6672611919923</v>
+        <v>42.87361574505626</v>
       </c>
       <c r="P10" t="n">
-        <v>4.132335337076729</v>
+        <v>585.4162428299137</v>
       </c>
       <c r="Q10" t="n">
-        <v>104.3740226137085</v>
+        <v>10.1482176774715</v>
       </c>
       <c r="R10" t="n">
-        <v>690.8474704773404</v>
+        <v>90.37442172330952</v>
       </c>
       <c r="S10" t="n">
-        <v>15.05098659295363</v>
+        <v>1916.17245028637</v>
       </c>
       <c r="T10" t="n">
-        <v>160.9027497932251</v>
+        <v>78</v>
       </c>
       <c r="U10" t="n">
-        <v>1343.231087538981</v>
+        <v>100</v>
       </c>
       <c r="V10" t="n">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="W10" t="n">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="X10" t="n">
-        <v>215</v>
+        <v>0.4742233923926838</v>
       </c>
       <c r="Y10" t="n">
-        <v>16</v>
+        <v>0.6235060810188122</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.5130578079877071</v>
+        <v>9.169547353982834</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.765305752643435</v>
+        <v>1126.606149250699</v>
       </c>
       <c r="AB10" t="n">
-        <v>55.41529261619298</v>
+        <v>129.1787232663497</v>
       </c>
       <c r="AC10" t="n">
-        <v>1934.953333700244</v>
+        <v>0.1449856362277236</v>
       </c>
       <c r="AD10" t="n">
-        <v>12.25228395614262</v>
+        <v>0.192611689422756</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.155301135358832</v>
+        <v>2.827102000603158</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.5291617607121967</v>
+        <v>143.9621991593577</v>
       </c>
       <c r="AG10" t="n">
-        <v>17.83755139688578</v>
+        <v>47.95483834169022</v>
       </c>
       <c r="AH10" t="n">
-        <v>76.93782025501758</v>
+        <v>265.5400906119252</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.1982684789237371</v>
+        <v>-2521.065280868095</v>
       </c>
       <c r="AJ10" t="n">
-        <v>-8846.013173548268</v>
+        <v>469.7461087459706</v>
       </c>
       <c r="AK10" t="n">
-        <v>-684.8218810907952</v>
+        <v>-1.485485756757001</v>
       </c>
       <c r="AL10" t="n">
-        <v>1297.132722220871</v>
+        <v>-8.478481267498989</v>
       </c>
       <c r="AM10" t="n">
-        <v>-1.822157777245562</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>-93.4212366608367</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>-523.1802092853482</v>
+        <v>-83.05080117559135</v>
       </c>
     </row>
     <row r="11">
@@ -1632,121 +1574,115 @@
         <v>20</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>103.1556357528465</v>
+        <v>102.1541506982907</v>
       </c>
       <c r="E11" t="n">
-        <v>11.0476089934037</v>
+        <v>10.74444456675616</v>
       </c>
       <c r="F11" t="n">
-        <v>115.4711489543338</v>
+        <v>113.8873821847502</v>
       </c>
       <c r="G11" t="n">
-        <v>2783.635862143582</v>
+        <v>2518.667495228005</v>
       </c>
       <c r="H11" t="n">
-        <v>430916.5774297701</v>
+        <v>451879.1252705344</v>
       </c>
       <c r="I11" t="n">
-        <v>456660.8491810913</v>
+        <v>470556.4834897429</v>
       </c>
       <c r="J11" t="n">
-        <v>-8896.665990386226</v>
+        <v>-25388.86847587764</v>
       </c>
       <c r="K11" t="n">
-        <v>8356.403123553539</v>
+        <v>0.1583116247330888</v>
       </c>
       <c r="L11" t="n">
-        <v>-5640.119118667785</v>
+        <v>4.240996840084542</v>
       </c>
       <c r="M11" t="n">
-        <v>2.706969021090718</v>
+        <v>158.7548319422687</v>
       </c>
       <c r="N11" t="n">
-        <v>10.90540297594377</v>
+        <v>6.666110903107523</v>
       </c>
       <c r="O11" t="n">
-        <v>137.786549849514</v>
+        <v>100.6808343794911</v>
       </c>
       <c r="P11" t="n">
-        <v>4.139854736010889</v>
+        <v>632.6046471971656</v>
       </c>
       <c r="Q11" t="n">
-        <v>104.3740226137085</v>
+        <v>10.58881480495952</v>
       </c>
       <c r="R11" t="n">
-        <v>940.8097827034992</v>
+        <v>152.925002778041</v>
       </c>
       <c r="S11" t="n">
-        <v>15.45529745314734</v>
+        <v>2017.406291342772</v>
       </c>
       <c r="T11" t="n">
-        <v>160.9027497932251</v>
+        <v>91</v>
       </c>
       <c r="U11" t="n">
-        <v>1690.057884137169</v>
+        <v>116</v>
       </c>
       <c r="V11" t="n">
-        <v>52</v>
+        <v>233</v>
       </c>
       <c r="W11" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="X11" t="n">
-        <v>235</v>
+        <v>0.522966818557287</v>
       </c>
       <c r="Y11" t="n">
-        <v>16</v>
+        <v>0.6867549734771164</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.5587206346595336</v>
+        <v>9.423075391251734</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.803289043464752</v>
+        <v>1258.567151344118</v>
       </c>
       <c r="AB11" t="n">
-        <v>55.82451597737123</v>
+        <v>177.6657118424732</v>
       </c>
       <c r="AC11" t="n">
-        <v>2153.713345081122</v>
+        <v>0.1604477552305837</v>
       </c>
       <c r="AD11" t="n">
-        <v>12.32011408459308</v>
+        <v>0.2111366830851858</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.1692365619181483</v>
+        <v>2.915896820659281</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.5424885349886576</v>
+        <v>184.5635986010419</v>
       </c>
       <c r="AG11" t="n">
-        <v>17.95996546313751</v>
+        <v>63.4427664010154</v>
       </c>
       <c r="AH11" t="n">
-        <v>157.5048657806736</v>
+        <v>485.133624955521</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.2179062287042456</v>
+        <v>280.7331541722525</v>
       </c>
       <c r="AJ11" t="n">
-        <v>765.140486061091</v>
+        <v>-877.0219952289403</v>
       </c>
       <c r="AK11" t="n">
-        <v>-128.9871226323794</v>
+        <v>-1.648947580938112</v>
       </c>
       <c r="AL11" t="n">
-        <v>-274.4020365633151</v>
+        <v>-15.00278199303987</v>
       </c>
       <c r="AM11" t="n">
-        <v>-1.432885714920171</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>-93.46861963776475</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>-803.0232328539852</v>
+        <v>-93.36243726238784</v>
       </c>
     </row>
     <row r="12">
@@ -1757,121 +1693,115 @@
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>103.4511450894512</v>
+        <v>102.6109398775664</v>
       </c>
       <c r="E12" t="n">
-        <v>11.1742040581588</v>
+        <v>10.83377496525806</v>
       </c>
       <c r="F12" t="n">
-        <v>117.0545293696283</v>
+        <v>113.7570112909131</v>
       </c>
       <c r="G12" t="n">
-        <v>2800.348115338365</v>
+        <v>2530.38886712224</v>
       </c>
       <c r="H12" t="n">
-        <v>430716.3947333698</v>
+        <v>454233.0736806333</v>
       </c>
       <c r="I12" t="n">
-        <v>454826.4609289135</v>
+        <v>474406.9789630602</v>
       </c>
       <c r="J12" t="n">
-        <v>-11099.02821406875</v>
+        <v>-26790.26436988042</v>
       </c>
       <c r="K12" t="n">
-        <v>8356.403123553539</v>
+        <v>-0.02176968056453742</v>
       </c>
       <c r="L12" t="n">
-        <v>-5640.119118667785</v>
+        <v>-17.72633230484027</v>
       </c>
       <c r="M12" t="n">
-        <v>2.720948453224691</v>
+        <v>80.5731393755315</v>
       </c>
       <c r="N12" t="n">
-        <v>6.07970241728728</v>
+        <v>6.213533114835149</v>
       </c>
       <c r="O12" t="n">
-        <v>208.9306683732895</v>
+        <v>106.6642474060374</v>
       </c>
       <c r="P12" t="n">
-        <v>4.294321778865859</v>
+        <v>630.6169625394674</v>
       </c>
       <c r="Q12" t="n">
-        <v>104.580407272961</v>
+        <v>10.83793480513014</v>
       </c>
       <c r="R12" t="n">
-        <v>1684.689578176801</v>
+        <v>140.7791634105501</v>
       </c>
       <c r="S12" t="n">
-        <v>15.62374392813629</v>
+        <v>2005.863336281092</v>
       </c>
       <c r="T12" t="n">
-        <v>162.7387958346683</v>
+        <v>103</v>
       </c>
       <c r="U12" t="n">
-        <v>2551.960772346254</v>
+        <v>127</v>
       </c>
       <c r="V12" t="n">
-        <v>56</v>
+        <v>261</v>
       </c>
       <c r="W12" t="n">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="X12" t="n">
-        <v>254</v>
+        <v>0.5807895551822225</v>
       </c>
       <c r="Y12" t="n">
-        <v>16</v>
+        <v>0.6018492785410418</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.5783529836651558</v>
+        <v>10.16854586931647</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.9037640275329</v>
+        <v>1511.225220069077</v>
       </c>
       <c r="AB12" t="n">
-        <v>70.22512377262332</v>
+        <v>185.8711658789437</v>
       </c>
       <c r="AC12" t="n">
-        <v>2234.676627635775</v>
+        <v>0.1785854140748573</v>
       </c>
       <c r="AD12" t="n">
-        <v>12.36731237330067</v>
+        <v>0.1834082966353685</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.1753719303288858</v>
+        <v>3.14242031572195</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.5730231830944646</v>
+        <v>301.1951093939107</v>
       </c>
       <c r="AG12" t="n">
-        <v>22.32977675950884</v>
+        <v>63.47045006275041</v>
       </c>
       <c r="AH12" t="n">
-        <v>187.4763622652678</v>
+        <v>155.0276500387981</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.2319447081764028</v>
+        <v>-108.2515917221833</v>
       </c>
       <c r="AJ12" t="n">
-        <v>212.6767105768393</v>
+        <v>221.3210752063551</v>
       </c>
       <c r="AK12" t="n">
-        <v>354.9526713672967</v>
+        <v>-1.227779276613074</v>
       </c>
       <c r="AL12" t="n">
-        <v>177.6258842856251</v>
+        <v>-23.028599633034</v>
       </c>
       <c r="AM12" t="n">
-        <v>-1.573373325641167</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>-98.50070485567372</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>-1475.758909803512</v>
+        <v>-130.9493278059539</v>
       </c>
     </row>
     <row r="13">
@@ -1882,121 +1812,115 @@
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>103.9158682090191</v>
+        <v>102.7668751492</v>
       </c>
       <c r="E13" t="n">
-        <v>11.09796118998313</v>
+        <v>10.8941894224786</v>
       </c>
       <c r="F13" t="n">
-        <v>117.2137552167309</v>
+        <v>112.947885997581</v>
       </c>
       <c r="G13" t="n">
-        <v>2927.693940799048</v>
+        <v>2529.672202113841</v>
       </c>
       <c r="H13" t="n">
-        <v>429314.0381771678</v>
+        <v>454703.3253272982</v>
       </c>
       <c r="I13" t="n">
-        <v>455423.0040134978</v>
+        <v>473870.8686667508</v>
       </c>
       <c r="J13" t="n">
-        <v>-8520.290483225288</v>
+        <v>-23673.5133520852</v>
       </c>
       <c r="K13" t="n">
-        <v>8356.403123553539</v>
+        <v>0.566163107270651</v>
       </c>
       <c r="L13" t="n">
-        <v>-5681.982903822082</v>
+        <v>-17.62492248664685</v>
       </c>
       <c r="M13" t="n">
-        <v>2.667605354472236</v>
+        <v>70.56008117572368</v>
       </c>
       <c r="N13" t="n">
-        <v>4.783888889573344</v>
+        <v>5.987507873806339</v>
       </c>
       <c r="O13" t="n">
-        <v>274.3308510216515</v>
+        <v>109.5189070852063</v>
       </c>
       <c r="P13" t="n">
-        <v>3.6207903639746</v>
+        <v>878.6096084139147</v>
       </c>
       <c r="Q13" t="n">
-        <v>111.7634211881287</v>
+        <v>11.5209433080046</v>
       </c>
       <c r="R13" t="n">
-        <v>1839.830996610325</v>
+        <v>152.9884796718227</v>
       </c>
       <c r="S13" t="n">
-        <v>15.64046536766604</v>
+        <v>2334.465974778566</v>
       </c>
       <c r="T13" t="n">
-        <v>170.202372667881</v>
+        <v>119</v>
       </c>
       <c r="U13" t="n">
-        <v>2876.700259372198</v>
+        <v>142</v>
       </c>
       <c r="V13" t="n">
-        <v>61</v>
+        <v>294</v>
       </c>
       <c r="W13" t="n">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="X13" t="n">
-        <v>271</v>
+        <v>0.6339289892240642</v>
       </c>
       <c r="Y13" t="n">
-        <v>17</v>
+        <v>0.6654251858996871</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.6000906815536942</v>
+        <v>10.28844243031238</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.951340188443482</v>
+        <v>1984.220974255246</v>
       </c>
       <c r="AB13" t="n">
-        <v>118.1044712080817</v>
+        <v>221.1812868470786</v>
       </c>
       <c r="AC13" t="n">
-        <v>2574.044868566723</v>
+        <v>0.1959847441859912</v>
       </c>
       <c r="AD13" t="n">
-        <v>19.84824209021642</v>
+        <v>0.2017494132436199</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.1819443221237476</v>
+        <v>3.178141401567638</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.5887384982514151</v>
+        <v>301.4840097170679</v>
       </c>
       <c r="AG13" t="n">
-        <v>36.85273555769282</v>
+        <v>63.60745895030919</v>
       </c>
       <c r="AH13" t="n">
-        <v>187.6202639341056</v>
+        <v>72.41219465679438</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.2569587153885485</v>
+        <v>-61.58370980989199</v>
       </c>
       <c r="AJ13" t="n">
-        <v>-1300.321154618119</v>
+        <v>582.0406229917896</v>
       </c>
       <c r="AK13" t="n">
-        <v>313.9040759697391</v>
+        <v>0.03027762198369438</v>
       </c>
       <c r="AL13" t="n">
-        <v>-403.6663789566096</v>
+        <v>-23.73221048232294</v>
       </c>
       <c r="AM13" t="n">
-        <v>-0.9531850095023636</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>-106.9795322985554</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>-1565.500145588674</v>
+        <v>-374.2683061646019</v>
       </c>
     </row>
     <row r="14">
@@ -2007,121 +1931,115 @@
         <v>20</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>104.1683590565673</v>
+        <v>103.039895963121</v>
       </c>
       <c r="E14" t="n">
-        <v>11.19757768160893</v>
+        <v>11.00077490389093</v>
       </c>
       <c r="F14" t="n">
-        <v>116.95572104648</v>
+        <v>113.0140687569275</v>
       </c>
       <c r="G14" t="n">
-        <v>2955.272099367726</v>
+        <v>2532.462856181338</v>
       </c>
       <c r="H14" t="n">
-        <v>428848.9311702812</v>
+        <v>450424.7827742068</v>
       </c>
       <c r="I14" t="n">
-        <v>458250.5844359481</v>
+        <v>478660.8606191596</v>
       </c>
       <c r="J14" t="n">
-        <v>-9850.524668890217</v>
+        <v>-23776.59883239843</v>
       </c>
       <c r="K14" t="n">
-        <v>7684.344425885022</v>
+        <v>0.3922134493724636</v>
       </c>
       <c r="L14" t="n">
-        <v>-6026.667321655103</v>
+        <v>-16.25809306085469</v>
       </c>
       <c r="M14" t="n">
-        <v>2.033111166590059</v>
+        <v>38.27289970362681</v>
       </c>
       <c r="N14" t="n">
-        <v>1.129283803165874</v>
+        <v>5.397263057743618</v>
       </c>
       <c r="O14" t="n">
-        <v>275.4943712858345</v>
+        <v>119.3093000544176</v>
       </c>
       <c r="P14" t="n">
-        <v>3.82527802692216</v>
+        <v>1192.437729907872</v>
       </c>
       <c r="Q14" t="n">
-        <v>80.33847636973034</v>
+        <v>11.92947633931533</v>
       </c>
       <c r="R14" t="n">
-        <v>1661.371845464084</v>
+        <v>172.3371291797128</v>
       </c>
       <c r="S14" t="n">
-        <v>16.21440357496616</v>
+        <v>2730.21229806788</v>
       </c>
       <c r="T14" t="n">
-        <v>177.2930394851322</v>
+        <v>130</v>
       </c>
       <c r="U14" t="n">
-        <v>2933.154546685271</v>
+        <v>155</v>
       </c>
       <c r="V14" t="n">
-        <v>66</v>
+        <v>327</v>
       </c>
       <c r="W14" t="n">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="X14" t="n">
-        <v>296</v>
+        <v>0.7111879742580665</v>
       </c>
       <c r="Y14" t="n">
-        <v>17</v>
+        <v>0.7620979577737967</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.65465954412276</v>
+        <v>10.53013455135642</v>
       </c>
       <c r="AA14" t="n">
-        <v>2.332493909106073</v>
+        <v>2698.491669137056</v>
       </c>
       <c r="AB14" t="n">
-        <v>118.3064905548928</v>
+        <v>282.1845909326588</v>
       </c>
       <c r="AC14" t="n">
-        <v>2977.093655808303</v>
+        <v>0.2198146379694023</v>
       </c>
       <c r="AD14" t="n">
-        <v>1233.246281277457</v>
+        <v>0.2296256565921985</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.1982601201081253</v>
+        <v>3.25116783775617</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.7031028806256104</v>
+        <v>301.7627901856271</v>
       </c>
       <c r="AG14" t="n">
-        <v>36.9136734455879</v>
+        <v>84.93960577577084</v>
       </c>
       <c r="AH14" t="n">
-        <v>188.3478835202585</v>
+        <v>189.7586435037988</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.382715635524955</v>
+        <v>-93.67221174460394</v>
       </c>
       <c r="AJ14" t="n">
-        <v>-26.72719966833074</v>
+        <v>580.5026498116695</v>
       </c>
       <c r="AK14" t="n">
-        <v>-387.3898247087</v>
+        <v>0.4950123803900962</v>
       </c>
       <c r="AL14" t="n">
-        <v>-459.6070043073946</v>
+        <v>-31.19309336809548</v>
       </c>
       <c r="AM14" t="n">
-        <v>-1.7921668603321</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>-79.20919256656447</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>-1385.87747417825</v>
+        <v>-711.1668221344762</v>
       </c>
     </row>
     <row r="15">
@@ -2132,121 +2050,115 @@
         <v>20</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>104.3199831739296</v>
+        <v>103.1905505147787</v>
       </c>
       <c r="E15" t="n">
-        <v>11.27108964057473</v>
+        <v>11.04037381189972</v>
       </c>
       <c r="F15" t="n">
-        <v>117.0113156033707</v>
+        <v>113.4235265545595</v>
       </c>
       <c r="G15" t="n">
-        <v>2961.87209453293</v>
+        <v>2538.322449990335</v>
       </c>
       <c r="H15" t="n">
-        <v>430415.6367554717</v>
+        <v>453103.1155917345</v>
       </c>
       <c r="I15" t="n">
-        <v>443779.5460337293</v>
+        <v>477739.2102767606</v>
       </c>
       <c r="J15" t="n">
-        <v>3769.564551976337</v>
+        <v>-26350.36697679007</v>
       </c>
       <c r="K15" t="n">
-        <v>9241.661958066472</v>
+        <v>-0.6648166378199385</v>
       </c>
       <c r="L15" t="n">
-        <v>-6215.490672364808</v>
+        <v>-17.2567022401792</v>
       </c>
       <c r="M15" t="n">
-        <v>2.105572818726099</v>
+        <v>62.59466869164049</v>
       </c>
       <c r="N15" t="n">
-        <v>3.838578254861097</v>
+        <v>6.134205272460222</v>
       </c>
       <c r="O15" t="n">
-        <v>275.4943712858345</v>
+        <v>123.5818022900174</v>
       </c>
       <c r="P15" t="n">
-        <v>3.103532339228783</v>
+        <v>964.3662343788715</v>
       </c>
       <c r="Q15" t="n">
-        <v>50.90949288806694</v>
+        <v>12.69231893137363</v>
       </c>
       <c r="R15" t="n">
-        <v>1622.137436337094</v>
+        <v>182.1207635480119</v>
       </c>
       <c r="S15" t="n">
-        <v>16.41954634361059</v>
+        <v>2784.275879987375</v>
       </c>
       <c r="T15" t="n">
-        <v>182.834542032186</v>
+        <v>141</v>
       </c>
       <c r="U15" t="n">
-        <v>2985.865328043223</v>
+        <v>169</v>
       </c>
       <c r="V15" t="n">
-        <v>71</v>
+        <v>356</v>
       </c>
       <c r="W15" t="n">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="X15" t="n">
-        <v>318</v>
+        <v>0.763029140095505</v>
       </c>
       <c r="Y15" t="n">
-        <v>18</v>
+        <v>0.8762867985919357</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.6882146060432046</v>
+        <v>10.58730165387437</v>
       </c>
       <c r="AA15" t="n">
-        <v>2.389186580694133</v>
+        <v>3251.205324578676</v>
       </c>
       <c r="AB15" t="n">
-        <v>118.3628120878523</v>
+        <v>282.2509250304352</v>
       </c>
       <c r="AC15" t="n">
-        <v>3342.787143637501</v>
+        <v>0.2351571531046344</v>
       </c>
       <c r="AD15" t="n">
-        <v>2388.050206180664</v>
+        <v>0.2637252257693598</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.2082210672004449</v>
+        <v>3.268429615542341</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.7200991081976834</v>
+        <v>302.5680988722939</v>
       </c>
       <c r="AG15" t="n">
-        <v>36.93067536519272</v>
+        <v>84.95959826253163</v>
       </c>
       <c r="AH15" t="n">
-        <v>188.4814501082333</v>
+        <v>-934.6785094452596</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.6606850494326472</v>
+        <v>-5.950326301456187</v>
       </c>
       <c r="AJ15" t="n">
-        <v>-25.5505805922119</v>
+        <v>92.67567258397526</v>
       </c>
       <c r="AK15" t="n">
-        <v>-11084.83596899487</v>
+        <v>-1.242745261375122</v>
       </c>
       <c r="AL15" t="n">
-        <v>362.9975814076965</v>
+        <v>-35.51744267296183</v>
       </c>
       <c r="AM15" t="n">
-        <v>-0.9979595205026831</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>-47.07091463320583</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>-1346.64306505126</v>
+        <v>-458.7735576174624</v>
       </c>
     </row>
     <row r="16">
@@ -2257,121 +2169,115 @@
         <v>20</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>104.8064828441859</v>
+        <v>103.366839657612</v>
       </c>
       <c r="E16" t="n">
-        <v>11.18551910179299</v>
+        <v>11.02772864907349</v>
       </c>
       <c r="F16" t="n">
-        <v>119.6341830128622</v>
+        <v>114.3059618800882</v>
       </c>
       <c r="G16" t="n">
-        <v>2930.052708477418</v>
+        <v>2558.998394449437</v>
       </c>
       <c r="H16" t="n">
-        <v>427158.8248169036</v>
+        <v>447319.5538530251</v>
       </c>
       <c r="I16" t="n">
-        <v>455308.2279756662</v>
+        <v>482421.5637025967</v>
       </c>
       <c r="J16" t="n">
-        <v>6681.108144567494</v>
+        <v>-26833.93994399816</v>
       </c>
       <c r="K16" t="n">
-        <v>9241.661958066472</v>
+        <v>-0.2481050939771984</v>
       </c>
       <c r="L16" t="n">
-        <v>-6182.813549431889</v>
+        <v>-19.54708813230705</v>
       </c>
       <c r="M16" t="n">
-        <v>1.904364386833313</v>
+        <v>136.9433084685137</v>
       </c>
       <c r="N16" t="n">
-        <v>3.838578254861097</v>
+        <v>5.92277759742158</v>
       </c>
       <c r="O16" t="n">
-        <v>249.1342263386369</v>
+        <v>125.199362391308</v>
       </c>
       <c r="P16" t="n">
-        <v>3.458710735542303</v>
+        <v>517.8620097034708</v>
       </c>
       <c r="Q16" t="n">
-        <v>36.06334551839133</v>
+        <v>13.14325033316785</v>
       </c>
       <c r="R16" t="n">
-        <v>1964.633155276272</v>
+        <v>185.5246589077715</v>
       </c>
       <c r="S16" t="n">
-        <v>16.94826012952413</v>
+        <v>2867.258637042155</v>
       </c>
       <c r="T16" t="n">
-        <v>183.3207600831597</v>
+        <v>159</v>
       </c>
       <c r="U16" t="n">
-        <v>3607.699159896598</v>
+        <v>179</v>
       </c>
       <c r="V16" t="n">
-        <v>72</v>
+        <v>383</v>
       </c>
       <c r="W16" t="n">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="X16" t="n">
-        <v>339</v>
+        <v>0.8214164992282951</v>
       </c>
       <c r="Y16" t="n">
-        <v>19</v>
+        <v>0.9518607309486</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.7162605774949214</v>
+        <v>10.70599014471833</v>
       </c>
       <c r="AA16" t="n">
-        <v>2.429297935927805</v>
+        <v>4040.797073417912</v>
       </c>
       <c r="AB16" t="n">
-        <v>119.0680397572448</v>
+        <v>310.8964008360721</v>
       </c>
       <c r="AC16" t="n">
-        <v>4132.982269023343</v>
+        <v>0.2525241800343199</v>
       </c>
       <c r="AD16" t="n">
-        <v>2676.1289961394</v>
+        <v>0.2865131404406464</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.2165866355750524</v>
+        <v>3.304316383845715</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.7355225324727503</v>
+        <v>303.9474683798321</v>
       </c>
       <c r="AG16" t="n">
-        <v>37.14231750433834</v>
+        <v>86.821197945414</v>
       </c>
       <c r="AH16" t="n">
-        <v>189.3517465734162</v>
+        <v>32.17990556312343</v>
       </c>
       <c r="AI16" t="n">
-        <v>95.08041151801982</v>
+        <v>-8.76065796601074</v>
       </c>
       <c r="AJ16" t="n">
-        <v>-26.0875043015547</v>
+        <v>2.546274710313015</v>
       </c>
       <c r="AK16" t="n">
-        <v>-988.2395466786008</v>
+        <v>-0.2917688087008574</v>
       </c>
       <c r="AL16" t="n">
-        <v>-78.52124409426239</v>
+        <v>-39.40685983344142</v>
       </c>
       <c r="AM16" t="n">
-        <v>-1.55434634870899</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>-32.22476726353023</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>-1715.498928937636</v>
+        <v>63.61924819977893</v>
       </c>
     </row>
     <row r="17">
@@ -2382,121 +2288,115 @@
         <v>20</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>105.1510860192137</v>
+        <v>103.5028035738255</v>
       </c>
       <c r="E17" t="n">
-        <v>11.20750554656695</v>
+        <v>11.09148499773197</v>
       </c>
       <c r="F17" t="n">
-        <v>119.6840112729881</v>
+        <v>114.3318573026558</v>
       </c>
       <c r="G17" t="n">
-        <v>2945.645919521848</v>
+        <v>2559.189614593322</v>
       </c>
       <c r="H17" t="n">
-        <v>422559.5439205884</v>
+        <v>447288.4627736189</v>
       </c>
       <c r="I17" t="n">
-        <v>461190.0451665798</v>
+        <v>483414.9811385078</v>
       </c>
       <c r="J17" t="n">
-        <v>10892.6725389039</v>
+        <v>-27846.01454814625</v>
       </c>
       <c r="K17" t="n">
-        <v>9241.661958066472</v>
+        <v>-1.063150424115451</v>
       </c>
       <c r="L17" t="n">
-        <v>-6182.813549431889</v>
+        <v>-18.96504297813395</v>
       </c>
       <c r="M17" t="n">
-        <v>1.911425410826855</v>
+        <v>193.4296829186875</v>
       </c>
       <c r="N17" t="n">
-        <v>4.064524880855704</v>
+        <v>6.941378809627421</v>
       </c>
       <c r="O17" t="n">
-        <v>292.2933432835289</v>
+        <v>117.8465710159306</v>
       </c>
       <c r="P17" t="n">
-        <v>8.671323329154644</v>
+        <v>979.8423007065294</v>
       </c>
       <c r="Q17" t="n">
-        <v>109.8881987424108</v>
+        <v>14.16243664171231</v>
       </c>
       <c r="R17" t="n">
-        <v>1965.633104527569</v>
+        <v>188.1200158853004</v>
       </c>
       <c r="S17" t="n">
-        <v>22.76978389190717</v>
+        <v>3389.980810867723</v>
       </c>
       <c r="T17" t="n">
-        <v>257.6588878275224</v>
+        <v>167</v>
       </c>
       <c r="U17" t="n">
-        <v>3774.77008310028</v>
+        <v>194</v>
       </c>
       <c r="V17" t="n">
-        <v>77</v>
+        <v>406</v>
       </c>
       <c r="W17" t="n">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="X17" t="n">
-        <v>353</v>
+        <v>0.8695590520326659</v>
       </c>
       <c r="Y17" t="n">
-        <v>19</v>
+        <v>1.00552614295321</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.7368034034387299</v>
+        <v>10.86709284298536</v>
       </c>
       <c r="AA17" t="n">
-        <v>2.463727288065493</v>
+        <v>4452.228979428628</v>
       </c>
       <c r="AB17" t="n">
-        <v>126.6022101946317</v>
+        <v>339.7046497287544</v>
       </c>
       <c r="AC17" t="n">
-        <v>4572.214458779136</v>
+        <v>0.2671594197446244</v>
       </c>
       <c r="AD17" t="n">
-        <v>2720.903142404973</v>
+        <v>0.3022605875452082</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.2228753668474353</v>
+        <v>3.352706600948989</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.752717128803711</v>
+        <v>303.9841126413004</v>
       </c>
       <c r="AG17" t="n">
-        <v>39.41735336963361</v>
+        <v>88.51770586377391</v>
       </c>
       <c r="AH17" t="n">
-        <v>189.7319594791019</v>
+        <v>54.32293851751155</v>
       </c>
       <c r="AI17" t="n">
-        <v>139.81875478728</v>
+        <v>0.5674634109908538</v>
       </c>
       <c r="AJ17" t="n">
-        <v>98.46799903614605</v>
+        <v>12.7779608205972</v>
       </c>
       <c r="AK17" t="n">
-        <v>190.3223237024057</v>
+        <v>-1.760474612015627</v>
       </c>
       <c r="AL17" t="n">
-        <v>19.66759079515657</v>
+        <v>-30.48019630290785</v>
       </c>
       <c r="AM17" t="n">
-        <v>-6.759897918327789</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>-105.8236738615551</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>-1673.339761244041</v>
+        <v>-320.1069474855922</v>
       </c>
     </row>
     <row r="18">
@@ -2507,121 +2407,115 @@
         <v>20</v>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>105.4583361101137</v>
+        <v>103.6297128948809</v>
       </c>
       <c r="E18" t="n">
-        <v>11.30480667314384</v>
+        <v>11.09196006778159</v>
       </c>
       <c r="F18" t="n">
-        <v>120.3428032254699</v>
+        <v>114.6299954374788</v>
       </c>
       <c r="G18" t="n">
-        <v>2942.942339825753</v>
+        <v>2558.759144488998</v>
       </c>
       <c r="H18" t="n">
-        <v>426032.203042427</v>
+        <v>448304.3110193665</v>
       </c>
       <c r="I18" t="n">
-        <v>464586.919783538</v>
+        <v>484386.8337713773</v>
       </c>
       <c r="J18" t="n">
-        <v>5877.454766573113</v>
+        <v>-28136.27270938157</v>
       </c>
       <c r="K18" t="n">
-        <v>9241.661958066472</v>
+        <v>-1.059559442639544</v>
       </c>
       <c r="L18" t="n">
-        <v>-11014.53888615015</v>
+        <v>-18.35820191670754</v>
       </c>
       <c r="M18" t="n">
-        <v>1.484990955892949</v>
+        <v>39.99105589005364</v>
       </c>
       <c r="N18" t="n">
-        <v>6.130604356139568</v>
+        <v>7.15944021554059</v>
       </c>
       <c r="O18" t="n">
-        <v>293.2429454206075</v>
+        <v>122.7096627044377</v>
       </c>
       <c r="P18" t="n">
-        <v>8.716770643726889</v>
+        <v>1124.916632474078</v>
       </c>
       <c r="Q18" t="n">
-        <v>112.5181110927218</v>
+        <v>14.46914265707002</v>
       </c>
       <c r="R18" t="n">
-        <v>1592.61608395684</v>
+        <v>193.7324913508663</v>
       </c>
       <c r="S18" t="n">
-        <v>22.98553862054242</v>
+        <v>3547.214383533268</v>
       </c>
       <c r="T18" t="n">
-        <v>264.2095556003704</v>
+        <v>175</v>
       </c>
       <c r="U18" t="n">
-        <v>3933.744433327053</v>
+        <v>209</v>
       </c>
       <c r="V18" t="n">
-        <v>81</v>
+        <v>427</v>
       </c>
       <c r="W18" t="n">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="X18" t="n">
-        <v>375</v>
+        <v>0.9221151539745901</v>
       </c>
       <c r="Y18" t="n">
-        <v>20</v>
+        <v>1.04590161405326</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.8032632812759934</v>
+        <v>12.12385111551943</v>
       </c>
       <c r="AA18" t="n">
-        <v>2.5319271835484</v>
+        <v>4484.013433947706</v>
       </c>
       <c r="AB18" t="n">
-        <v>127.6309451107402</v>
+        <v>339.8709408385934</v>
       </c>
       <c r="AC18" t="n">
-        <v>5366.818927891022</v>
+        <v>0.2829648121065578</v>
       </c>
       <c r="AD18" t="n">
-        <v>2865.178003659143</v>
+        <v>0.3143424148213159</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.2427609469346331</v>
+        <v>3.73508664367715</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.7738608239271449</v>
+        <v>304.035894490875</v>
       </c>
       <c r="AG18" t="n">
-        <v>39.7264687835434</v>
+        <v>88.53130601820658</v>
       </c>
       <c r="AH18" t="n">
-        <v>191.323388738112</v>
+        <v>-11.86488964811099</v>
       </c>
       <c r="AI18" t="n">
-        <v>171.3525407936083</v>
+        <v>42.31798682941087</v>
       </c>
       <c r="AJ18" t="n">
-        <v>-26.50468750044246</v>
+        <v>16.68483911475801</v>
       </c>
       <c r="AK18" t="n">
-        <v>-215.3884536823373</v>
+        <v>-1.963982693373878</v>
       </c>
       <c r="AL18" t="n">
-        <v>-53.40404699791452</v>
+        <v>-33.07910879530236</v>
       </c>
       <c r="AM18" t="n">
-        <v>-7.23177968783394</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>-106.3875067365822</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>-1299.373138536233</v>
+        <v>-490.104755030703</v>
       </c>
     </row>
     <row r="19">
@@ -2632,121 +2526,115 @@
         <v>20</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19" t="n">
-        <v>105.7235307386951</v>
+        <v>103.7828684672084</v>
       </c>
       <c r="E19" t="n">
-        <v>11.32481896906493</v>
+        <v>11.13787078384529</v>
       </c>
       <c r="F19" t="n">
-        <v>120.9779787503647</v>
+        <v>114.5836791160177</v>
       </c>
       <c r="G19" t="n">
-        <v>2946.314025455059</v>
+        <v>2569.003118644172</v>
       </c>
       <c r="H19" t="n">
-        <v>420626.0912757341</v>
+        <v>450963.1461929597</v>
       </c>
       <c r="I19" t="n">
-        <v>471948.221831174</v>
+        <v>483650.5171680038</v>
       </c>
       <c r="J19" t="n">
-        <v>7750.223330400864</v>
+        <v>-30121.82712733743</v>
       </c>
       <c r="K19" t="n">
-        <v>9241.661958066472</v>
+        <v>-1.421591691372126</v>
       </c>
       <c r="L19" t="n">
-        <v>-11014.53888615015</v>
+        <v>-20.17430742567997</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2899734651093345</v>
+        <v>19.94884098158248</v>
       </c>
       <c r="N19" t="n">
-        <v>7.155908948800151</v>
+        <v>6.593040005678319</v>
       </c>
       <c r="O19" t="n">
-        <v>292.505742499525</v>
+        <v>106.382774798836</v>
       </c>
       <c r="P19" t="n">
-        <v>10.05571246168115</v>
+        <v>1387.514777930911</v>
       </c>
       <c r="Q19" t="n">
-        <v>91.49527869424621</v>
+        <v>14.71463173036978</v>
       </c>
       <c r="R19" t="n">
-        <v>1411.731622857</v>
+        <v>192.1604385381005</v>
       </c>
       <c r="S19" t="n">
-        <v>24.48530371424424</v>
+        <v>3885.403207183153</v>
       </c>
       <c r="T19" t="n">
-        <v>266.1860974651286</v>
+        <v>192</v>
       </c>
       <c r="U19" t="n">
-        <v>3933.744433327053</v>
+        <v>220</v>
       </c>
       <c r="V19" t="n">
-        <v>82</v>
+        <v>447</v>
       </c>
       <c r="W19" t="n">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="X19" t="n">
-        <v>393</v>
+        <v>0.9726627931584978</v>
       </c>
       <c r="Y19" t="n">
-        <v>20</v>
+        <v>1.058856867760434</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.8317839172286636</v>
+        <v>12.24684356290333</v>
       </c>
       <c r="AA19" t="n">
-        <v>2.588009463573751</v>
+        <v>5452.147893045052</v>
       </c>
       <c r="AB19" t="n">
-        <v>127.6844831029128</v>
+        <v>346.2568935282927</v>
       </c>
       <c r="AC19" t="n">
-        <v>6396.837889613683</v>
+        <v>0.2979590309465739</v>
       </c>
       <c r="AD19" t="n">
-        <v>2915.720160237379</v>
+        <v>0.3185448221246817</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.2511845782419843</v>
+        <v>3.772464430146733</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.7909193305485599</v>
+        <v>304.2974119195387</v>
       </c>
       <c r="AG19" t="n">
-        <v>39.74264476017738</v>
+        <v>88.56273620681903</v>
       </c>
       <c r="AH19" t="n">
-        <v>191.951673278682</v>
+        <v>-190.1137368238551</v>
       </c>
       <c r="AI19" t="n">
-        <v>221.8665761274938</v>
+        <v>17.66312372090812</v>
       </c>
       <c r="AJ19" t="n">
-        <v>455.931852054337</v>
+        <v>-152.9156111908453</v>
       </c>
       <c r="AK19" t="n">
-        <v>-1945.570303324741</v>
+        <v>-1.708143159482424</v>
       </c>
       <c r="AL19" t="n">
-        <v>-36.93886887526351</v>
+        <v>-16.0460329906012</v>
       </c>
       <c r="AM19" t="n">
-        <v>-9.765738996571812</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>-84.33936974544604</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>-1119.225880357475</v>
+        <v>-751.6421383322572</v>
       </c>
     </row>
     <row r="20">
@@ -2757,121 +2645,115 @@
         <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" t="n">
-        <v>105.9018687220079</v>
+        <v>103.9142923901194</v>
       </c>
       <c r="E20" t="n">
-        <v>11.3143613433062</v>
+        <v>11.06593596631541</v>
       </c>
       <c r="F20" t="n">
-        <v>121.5903216482443</v>
+        <v>114.6121852090516</v>
       </c>
       <c r="G20" t="n">
-        <v>2923.22379607985</v>
+        <v>2547.169881096374</v>
       </c>
       <c r="H20" t="n">
-        <v>414509.2657992952</v>
+        <v>456134.8345994006</v>
       </c>
       <c r="I20" t="n">
-        <v>472380.1801043245</v>
+        <v>488255.0551310779</v>
       </c>
       <c r="J20" t="n">
-        <v>20715.24725150369</v>
+        <v>-31370.80556476877</v>
       </c>
       <c r="K20" t="n">
-        <v>9960.143816495853</v>
+        <v>-1.458909623287447</v>
       </c>
       <c r="L20" t="n">
-        <v>-11014.53888615015</v>
+        <v>-30.14937023602711</v>
       </c>
       <c r="M20" t="n">
-        <v>0.3932734883226719</v>
+        <v>163.6175864063645</v>
       </c>
       <c r="N20" t="n">
-        <v>6.657246514898213</v>
+        <v>6.952920627330372</v>
       </c>
       <c r="O20" t="n">
-        <v>223.382772144116</v>
+        <v>106.7725733033162</v>
       </c>
       <c r="P20" t="n">
-        <v>10.77434788015484</v>
+        <v>1534.498346010907</v>
       </c>
       <c r="Q20" t="n">
-        <v>87.98347599691307</v>
+        <v>15.12611004916181</v>
       </c>
       <c r="R20" t="n">
-        <v>717.4811973794816</v>
+        <v>184.9742234360464</v>
       </c>
       <c r="S20" t="n">
-        <v>25.56541257287164</v>
+        <v>4200.767646894911</v>
       </c>
       <c r="T20" t="n">
-        <v>279.4098839918822</v>
+        <v>200</v>
       </c>
       <c r="U20" t="n">
-        <v>3934.114636363275</v>
+        <v>236</v>
       </c>
       <c r="V20" t="n">
-        <v>84</v>
+        <v>476</v>
       </c>
       <c r="W20" t="n">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="X20" t="n">
-        <v>414</v>
+        <v>1.034018200812064</v>
       </c>
       <c r="Y20" t="n">
-        <v>21</v>
+        <v>1.027253173951742</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.8695223180100264</v>
+        <v>12.80268489363586</v>
       </c>
       <c r="AA20" t="n">
-        <v>2.694821640929847</v>
+        <v>5454.707692934654</v>
       </c>
       <c r="AB20" t="n">
-        <v>128.4224131337716</v>
+        <v>351.7880015215553</v>
       </c>
       <c r="AC20" t="n">
-        <v>7935.398940991999</v>
+        <v>0.3172046412163378</v>
       </c>
       <c r="AD20" t="n">
-        <v>2975.961947835205</v>
+        <v>0.3094820157119754</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.2624113901621055</v>
+        <v>3.938400137389138</v>
       </c>
       <c r="AF20" t="n">
-        <v>0.8233084400803387</v>
+        <v>304.3234815155797</v>
       </c>
       <c r="AG20" t="n">
-        <v>39.96420565459417</v>
+        <v>88.58368499190948</v>
       </c>
       <c r="AH20" t="n">
-        <v>194.0405088787545</v>
+        <v>-198.5245750946245</v>
       </c>
       <c r="AI20" t="n">
-        <v>222.1733249580328</v>
+        <v>1412.411315287995</v>
       </c>
       <c r="AJ20" t="n">
-        <v>49.66633342142268</v>
+        <v>30.20069679947164</v>
       </c>
       <c r="AK20" t="n">
-        <v>-1198.154746107196</v>
+        <v>-2.137507279885269</v>
       </c>
       <c r="AL20" t="n">
-        <v>-1065.57633888949</v>
+        <v>-18.69327342876627</v>
       </c>
       <c r="AM20" t="n">
-        <v>-10.38107439183217</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>-81.32622948201484</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>-494.0984252353658</v>
+        <v>-888.6242315268141</v>
       </c>
     </row>
     <row r="21">
@@ -2882,121 +2764,115 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>106.0077226452962</v>
+        <v>104.0801277579057</v>
       </c>
       <c r="E21" t="n">
-        <v>11.34315215242731</v>
+        <v>11.12919160199701</v>
       </c>
       <c r="F21" t="n">
-        <v>122.1588728914166</v>
+        <v>113.8135388108608</v>
       </c>
       <c r="G21" t="n">
-        <v>2925.759178820526</v>
+        <v>2557.960810055117</v>
       </c>
       <c r="H21" t="n">
-        <v>412725.172556477</v>
+        <v>458142.5706133089</v>
       </c>
       <c r="I21" t="n">
-        <v>473132.6122854883</v>
+        <v>488297.9667476661</v>
       </c>
       <c r="J21" t="n">
-        <v>21007.65298313052</v>
+        <v>-31635.04264717796</v>
       </c>
       <c r="K21" t="n">
-        <v>9960.143816495853</v>
+        <v>-1.262875626156105</v>
       </c>
       <c r="L21" t="n">
-        <v>-11014.53888615015</v>
+        <v>-30.46195792056629</v>
       </c>
       <c r="M21" t="n">
-        <v>0.3932734883226719</v>
+        <v>149.8091678533978</v>
       </c>
       <c r="N21" t="n">
-        <v>3.912276309701314</v>
+        <v>6.590959062844884</v>
       </c>
       <c r="O21" t="n">
-        <v>104.5928114342752</v>
+        <v>107.8844280828911</v>
       </c>
       <c r="P21" t="n">
-        <v>10.92640946081432</v>
+        <v>1458.32884436532</v>
       </c>
       <c r="Q21" t="n">
-        <v>86.93638356669304</v>
+        <v>15.3483027543786</v>
       </c>
       <c r="R21" t="n">
-        <v>692.4970836181453</v>
+        <v>186.2530150849861</v>
       </c>
       <c r="S21" t="n">
-        <v>25.71747415353112</v>
+        <v>4264.059883695879</v>
       </c>
       <c r="T21" t="n">
-        <v>278.5590879127592</v>
+        <v>211</v>
       </c>
       <c r="U21" t="n">
-        <v>3981.881203441066</v>
+        <v>251</v>
       </c>
       <c r="V21" t="n">
-        <v>86</v>
+        <v>502</v>
       </c>
       <c r="W21" t="n">
-        <v>172</v>
+        <v>78</v>
       </c>
       <c r="X21" t="n">
-        <v>428</v>
+        <v>1.085720044669822</v>
       </c>
       <c r="Y21" t="n">
-        <v>22</v>
+        <v>1.080129127194329</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.8907688130808764</v>
+        <v>13.16482887990667</v>
       </c>
       <c r="AA21" t="n">
-        <v>2.756515674509219</v>
+        <v>5788.04020824006</v>
       </c>
       <c r="AB21" t="n">
-        <v>129.6427437568954</v>
+        <v>356.8551088460757</v>
       </c>
       <c r="AC21" t="n">
-        <v>8052.715627158245</v>
+        <v>0.3318972315443779</v>
       </c>
       <c r="AD21" t="n">
-        <v>2976.018723781858</v>
+        <v>0.3270403342293041</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.2687236210446607</v>
+        <v>4.044623186468647</v>
       </c>
       <c r="AF21" t="n">
-        <v>0.8421051740212846</v>
+        <v>317.1851665283024</v>
       </c>
       <c r="AG21" t="n">
-        <v>40.33140743435089</v>
+        <v>88.59758713710761</v>
       </c>
       <c r="AH21" t="n">
-        <v>214.2084904019549</v>
+        <v>-370.2984523863299</v>
       </c>
       <c r="AI21" t="n">
-        <v>222.1898126818125</v>
+        <v>20.43632446583763</v>
       </c>
       <c r="AJ21" t="n">
-        <v>145.0646890014577</v>
+        <v>-131.6667575971601</v>
       </c>
       <c r="AK21" t="n">
-        <v>0.6623299660400335</v>
+        <v>-1.55425180841431</v>
       </c>
       <c r="AL21" t="n">
-        <v>-847.8387799629936</v>
+        <v>-19.03270008562581</v>
       </c>
       <c r="AM21" t="n">
-        <v>-10.53313597249164</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>-83.0241072569917</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>-587.9042721838704</v>
+        <v>-820.8571016680014</v>
       </c>
     </row>
     <row r="22">
@@ -3007,121 +2883,115 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22" t="n">
-        <v>106.1549270962739</v>
+        <v>104.3346351744085</v>
       </c>
       <c r="E22" t="n">
-        <v>11.34607091047242</v>
+        <v>11.30975503963886</v>
       </c>
       <c r="F22" t="n">
-        <v>122.6087980429151</v>
+        <v>114.2492870863051</v>
       </c>
       <c r="G22" t="n">
-        <v>2929.633150246637</v>
+        <v>2563.933119006824</v>
       </c>
       <c r="H22" t="n">
-        <v>404760.3562233775</v>
+        <v>454533.6582345346</v>
       </c>
       <c r="I22" t="n">
-        <v>481696.9567218355</v>
+        <v>487535.5138936783</v>
       </c>
       <c r="J22" t="n">
-        <v>23735.33008252746</v>
+        <v>-31685.99954082584</v>
       </c>
       <c r="K22" t="n">
-        <v>9856.315100814203</v>
+        <v>-1.258736698509748</v>
       </c>
       <c r="L22" t="n">
-        <v>-9161.598642002347</v>
+        <v>-31.09050154814122</v>
       </c>
       <c r="M22" t="n">
-        <v>0.3137308643333981</v>
+        <v>95.28342025936013</v>
       </c>
       <c r="N22" t="n">
-        <v>4.717247185900745</v>
+        <v>7.045194968774501</v>
       </c>
       <c r="O22" t="n">
-        <v>117.521725793788</v>
+        <v>138.8385187943632</v>
       </c>
       <c r="P22" t="n">
-        <v>8.882998328148407</v>
+        <v>1572.732646456509</v>
       </c>
       <c r="Q22" t="n">
-        <v>58.53739374040748</v>
+        <v>16.01902228146692</v>
       </c>
       <c r="R22" t="n">
-        <v>843.7175586364804</v>
+        <v>220.3306212738403</v>
       </c>
       <c r="S22" t="n">
-        <v>25.71747415353112</v>
+        <v>4341.821152477276</v>
       </c>
       <c r="T22" t="n">
-        <v>283.1689964045165</v>
+        <v>227</v>
       </c>
       <c r="U22" t="n">
-        <v>4151.720280517797</v>
+        <v>266</v>
       </c>
       <c r="V22" t="n">
-        <v>91</v>
+        <v>526</v>
       </c>
       <c r="W22" t="n">
-        <v>179</v>
+        <v>83</v>
       </c>
       <c r="X22" t="n">
-        <v>439</v>
+        <v>1.19301226244078</v>
       </c>
       <c r="Y22" t="n">
-        <v>24</v>
+        <v>1.109805789849841</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.9080343975415877</v>
+        <v>13.39047505712402</v>
       </c>
       <c r="AA22" t="n">
-        <v>2.851704947335361</v>
+        <v>5898.833313147759</v>
       </c>
       <c r="AB22" t="n">
-        <v>131.1088069750212</v>
+        <v>358.9510198964631</v>
       </c>
       <c r="AC22" t="n">
-        <v>9294.142455256082</v>
+        <v>0.362252755475695</v>
       </c>
       <c r="AD22" t="n">
-        <v>3547.426899624077</v>
+        <v>0.3374686250558122</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.273463424344912</v>
+        <v>4.111808911932927</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.8710177872795279</v>
+        <v>327.4645376146351</v>
       </c>
       <c r="AG22" t="n">
-        <v>40.7721443218597</v>
+        <v>88.61437963149113</v>
       </c>
       <c r="AH22" t="n">
-        <v>214.3071880028748</v>
+        <v>-92.15534297391218</v>
       </c>
       <c r="AI22" t="n">
-        <v>222.206494218649</v>
+        <v>13.55380241424609</v>
       </c>
       <c r="AJ22" t="n">
-        <v>-5487.778125233489</v>
+        <v>-1671.276423669221</v>
       </c>
       <c r="AK22" t="n">
-        <v>-75.98910205491165</v>
+        <v>-1.868828328200577</v>
       </c>
       <c r="AL22" t="n">
-        <v>-1169.720021379941</v>
+        <v>-50.01836866458946</v>
       </c>
       <c r="AM22" t="n">
-        <v>-8.569267463815008</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>-53.82014655450669</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>-726.1958328426927</v>
+        <v>-831.2390435135956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>